<commit_message>
20230223:modified screen of SDWe , but not add varible
</commit_message>
<xml_diff>
--- a/SoftWare/SDWe/SDWe注意事项.xlsx
+++ b/SoftWare/SDWe/SDWe注意事项.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\GitWorkSpace\TBES_2022\SoftWare\SDWe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB3722E-F8C9-4316-B75F-97DE099484F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2900FD7-FB4B-46EA-8390-7FD109FF95C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,9 +24,22 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>0.ZDK比较特殊：可以设置2~128大小字体，(#`O′未加粗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果想用其他大小，且加粗字体，就得生成对应字库，且数据变量的‘Y方向点阵数’要和新的字库封装大小一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -39,6 +52,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -62,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -393,14 +414,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A33:A36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AA33" sqref="AA33"/>
+      <selection activeCell="Z43" sqref="Z43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="33" spans="1:1" ht="35.25" x14ac:dyDescent="0.5">
+      <c r="A33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="35.25" x14ac:dyDescent="0.5">
+      <c r="A36" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
liusu sample at use middle weight
</commit_message>
<xml_diff>
--- a/SoftWare/SDWe/SDWe注意事项.xlsx
+++ b/SoftWare/SDWe/SDWe注意事项.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\GitWorkSpace\TBES_2022\SoftWare\SDWe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2900FD7-FB4B-46EA-8390-7FD109FF95C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C5714F-AE25-4380-9802-BAF151468960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>0.ZDK比较特殊：可以设置2~128大小字体，(#`O′未加粗</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,12 +34,16 @@
     <t>如果想用其他大小，且加粗字体，就得生成对应字库，且数据变量的‘Y方向点阵数’要和新的字库封装大小一致</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>如果出现下载时CRC错误，可以删除VT_SET下的CheckSum.bin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +60,13 @@
     </font>
     <font>
       <sz val="28"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
       <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="2"/>
@@ -82,9 +93,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -414,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A33:A36"/>
+  <dimension ref="A33:A41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z43" sqref="Z43"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -432,6 +444,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="41" spans="1:1" ht="30" x14ac:dyDescent="0.4">
+      <c r="A41" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>